<commit_message>
the basics of some scripts for the feedback session
</commit_message>
<xml_diff>
--- a/2018_2019/Tests/Test 3 solutions/IEP scores 20182019 test 3.xlsx
+++ b/2018_2019/Tests/Test 3 solutions/IEP scores 20182019 test 3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23250" yWindow="0" windowWidth="2610" windowHeight="7005"/>
+    <workbookView xWindow="25110" yWindow="0" windowWidth="2610" windowHeight="7005"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -934,8 +934,8 @@
   <dimension ref="A1:AX66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA61" sqref="AA61"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>